<commit_message>
create dirs and arrange files
</commit_message>
<xml_diff>
--- a/items_list.xlsx
+++ b/items_list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27706"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="68" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E58EB4A2-6203-4DC5-9742-F0368B075A86}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE7C8EC0-14E5-48EB-9F17-7E130E140D04}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -34,9 +34,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
-  <si>
-    <t>Item</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+  <si>
+    <t>Item_Name</t>
+  </si>
+  <si>
+    <t>Items</t>
   </si>
   <si>
     <t>Weights</t>
@@ -45,6 +48,9 @@
     <t>Price</t>
   </si>
   <si>
+    <t>Jeera</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಜೀರಿಗೆ </t>
   </si>
   <si>
@@ -54,6 +60,9 @@
     <t>10,20,30</t>
   </si>
   <si>
+    <t>Musturd</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಸಾಸಿವೆ </t>
   </si>
   <si>
@@ -63,6 +72,9 @@
     <t>10,20,31</t>
   </si>
   <si>
+    <t>Ground nut</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಶೇಂಗಾ </t>
   </si>
   <si>
@@ -72,6 +84,9 @@
     <t>10,20,32</t>
   </si>
   <si>
+    <t>Fried gram</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಪುಠಾಣಿ </t>
   </si>
   <si>
@@ -81,6 +96,9 @@
     <t>10,20,33</t>
   </si>
   <si>
+    <t>Ragi</t>
+  </si>
+  <si>
     <t>ರಾಗಿ</t>
   </si>
   <si>
@@ -90,6 +108,9 @@
     <t>10,20,34</t>
   </si>
   <si>
+    <t>green peas</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಹಸಿರು  ವಠಾಣಿ </t>
   </si>
   <si>
@@ -99,6 +120,9 @@
     <t>10,20,35</t>
   </si>
   <si>
+    <t>white peas</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಬಿಳಿ  ವಠಾಣಿ </t>
   </si>
   <si>
@@ -108,6 +132,9 @@
     <t>10,20,36</t>
   </si>
   <si>
+    <t>Agasi seeds</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಅಗಸಿ </t>
   </si>
   <si>
@@ -117,6 +144,9 @@
     <t>10,20,37</t>
   </si>
   <si>
+    <t>Ajwain</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಅಜ್ವೈನ್ </t>
   </si>
   <si>
@@ -126,6 +156,9 @@
     <t>10,20,38</t>
   </si>
   <si>
+    <t>Alvi</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಆಳ್ವಿ </t>
   </si>
   <si>
@@ -135,6 +168,9 @@
     <t>10,20,39</t>
   </si>
   <si>
+    <t>Rice Flour</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಅಕ್ಕಿ  ಹಿಟ್ಟು </t>
   </si>
   <si>
@@ -144,6 +180,9 @@
     <t>10,20,40</t>
   </si>
   <si>
+    <t>Ragi Flour</t>
+  </si>
+  <si>
     <t xml:space="preserve">ರಾಗಿ  ಹಿಟ್ಟು </t>
   </si>
   <si>
@@ -153,6 +192,9 @@
     <t>10,20,41</t>
   </si>
   <si>
+    <t>Jawar Flour</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಜೋಳದ  ಹಿಟ್ಟು </t>
   </si>
   <si>
@@ -162,6 +204,9 @@
     <t>10,20,42</t>
   </si>
   <si>
+    <t>Antu</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಅಂಟು </t>
   </si>
   <si>
@@ -171,6 +216,9 @@
     <t>10,20,43</t>
   </si>
   <si>
+    <t>Badam</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಬದಾಮ್ </t>
   </si>
   <si>
@@ -180,6 +228,9 @@
     <t>10,20,44</t>
   </si>
   <si>
+    <t>Baking soda</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಅಡುಗೆ  ಸೋಡಾ </t>
   </si>
   <si>
@@ -189,6 +240,9 @@
     <t>10,20,45</t>
   </si>
   <si>
+    <t>Chana</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಕಡಲೆ  ಕಾಳು </t>
   </si>
   <si>
@@ -198,6 +252,9 @@
     <t>10,20,46</t>
   </si>
   <si>
+    <t>Chana dal</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಕಡಲೆ  ಬೇಳೆ </t>
   </si>
   <si>
@@ -207,6 +264,9 @@
     <t>10,20,47</t>
   </si>
   <si>
+    <t>chana Flour</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಕಡಲೆ  ಹಿಟ್ಟು </t>
   </si>
   <si>
@@ -216,6 +276,9 @@
     <t>10,20,48</t>
   </si>
   <si>
+    <t>Turmuric powder</t>
+  </si>
+  <si>
     <t xml:space="preserve">ಅರಿಶಿನ  ಪುಡಿ </t>
   </si>
   <si>
@@ -223,6 +286,9 @@
   </si>
   <si>
     <t>10,20,49</t>
+  </si>
+  <si>
+    <t>Pepper</t>
   </si>
   <si>
     <t xml:space="preserve">ಕಾಳು ಮೆಣಸು </t>
@@ -627,20 +693,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -650,240 +717,306 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>30</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="16.5" customHeight="1">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="16.5" customHeight="1">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>50</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>62</v>
+      </c>
+      <c r="D16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>70</v>
+      </c>
+      <c r="D18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>74</v>
+      </c>
+      <c r="D19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>82</v>
+      </c>
+      <c r="D21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>86</v>
+      </c>
+      <c r="D22" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="B1:D1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>